<commit_message>
Make tweet query properties consistent with ontology properties
</commit_message>
<xml_diff>
--- a/Agent/tweet_db.xlsx
+++ b/Agent/tweet_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hibaa\Documents\UU\Year 1\Q1\Intelligent Agents\IA\Agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEF5CF2-F4DF-431B-A377-2899B57B69B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FC8A75-F438-4C38-ADFD-C0231A01834C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>UserID</t>
   </si>
@@ -48,10 +48,6 @@
   </si>
   <si>
     <t>"@bigfatsurprise"</t>
-  </si>
-  <si>
-    <t>Does eating cake, cookies &amp; sweets cause breast cancer?
-There is no evidence that sugar consumption causes breast cancer - or any other type of cancer. It is true that being overweight can increase your breast cancer risk. Avoiding sugary foods is better for your health!</t>
   </si>
   <si>
     <t>"@wellness_hc"</t>
@@ -116,146 +112,141 @@
     <t>"@WebMD"</t>
   </si>
   <si>
+    <t>"@drdenwalker"</t>
+  </si>
+  <si>
+    <t>Research shows that a Mediterranean-style diet rich in fish, whole grains, green leafy vegetables, olives, and nuts helps maintain brain health and may reduce the risk of Alzheimer’s disease.</t>
+  </si>
+  <si>
+    <t>"@VitaminsMemory"</t>
+  </si>
+  <si>
+    <t>"@thehealthbot"</t>
+  </si>
+  <si>
+    <t>A lack of the right #nutrients including #vitamins A, C, D and E, #zinc, B vitamins, #iron, #biotin, #protein and essential fatty acids may slow down hair growth or even cause hair loss.</t>
+  </si>
+  <si>
+    <t>"@recipeiq"</t>
+  </si>
+  <si>
+    <t>predecessor atom</t>
+  </si>
+  <si>
+    <t>relation</t>
+  </si>
+  <si>
+    <t>cancer</t>
+  </si>
+  <si>
+    <t>cookies, candy, crackers, cereals</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>obesity</t>
+  </si>
+  <si>
+    <t>joints</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>shoulder pain</t>
+  </si>
+  <si>
+    <t>korean food</t>
+  </si>
+  <si>
+    <t>cream</t>
+  </si>
+  <si>
+    <t>sports AND uses-upper-body-parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eggs, meat </t>
+  </si>
+  <si>
+    <t>swimming</t>
+  </si>
+  <si>
+    <t>red meat</t>
+  </si>
+  <si>
+    <t>isA</t>
+  </si>
+  <si>
+    <t>kimbap, rabokki</t>
+  </si>
+  <si>
+    <t>carbonara</t>
+  </si>
+  <si>
+    <t>Alzheimers</t>
+  </si>
+  <si>
+    <t>nuts, blueberries, strawberries</t>
+  </si>
+  <si>
+    <t>cancer, Alzheimers</t>
+  </si>
+  <si>
+    <t>nuts, olive oil, cococunt oil</t>
+  </si>
+  <si>
+    <t>fish, whole grains, green leafy vegetables, olives, nuts</t>
+  </si>
+  <si>
+    <t>alcohol, obesity, no-sport, tobacco</t>
+  </si>
+  <si>
+    <t>lowVitamin</t>
+  </si>
+  <si>
+    <t>hairLoss</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>successor atom</t>
+  </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>Does eating cake, cookies &amp; sweets cause breast cancer?
+There is no evidence that sugar consumption causesCondition breast cancer - or any other type of cancer. It is true that being overweight can increase your breast cancer risk. Avoiding sugary foods is better for your health!</t>
+  </si>
+  <si>
+    <t>causesCondition</t>
+  </si>
+  <si>
     <t>Reasons why you should include Nuts, Seeds, Olive Oil, Coconut Oil
 •Normalizes Omega 3/6/9 fat ratios
 •Promotes healthy blood flow
-•Reduces body inflammation that causes heart attacks, Alzheimer’s and cancer to name a few
+•Reduces body inflammation that causesCondition heart attacks, Alzheimer’s and cancer to name a few
 RT and Share</t>
   </si>
   <si>
-    <t>"@drdenwalker"</t>
-  </si>
-  <si>
-    <t>Research shows that a Mediterranean-style diet rich in fish, whole grains, green leafy vegetables, olives, and nuts helps maintain brain health and may reduce the risk of Alzheimer’s disease.</t>
-  </si>
-  <si>
-    <t>"@VitaminsMemory"</t>
-  </si>
-  <si>
-    <t>Alcohol, obesity and physical inactivity are all preventable causes of cancer along with tobacco.</t>
-  </si>
-  <si>
-    <t>"@thehealthbot"</t>
-  </si>
-  <si>
-    <t>A lack of the right #nutrients including #vitamins A, C, D and E, #zinc, B vitamins, #iron, #biotin, #protein and essential fatty acids may slow down hair growth or even cause hair loss.</t>
-  </si>
-  <si>
-    <t>"@recipeiq"</t>
-  </si>
-  <si>
-    <t>predecessor atom</t>
-  </si>
-  <si>
-    <t>relation</t>
-  </si>
-  <si>
-    <t>cause</t>
-  </si>
-  <si>
-    <t>cancer</t>
-  </si>
-  <si>
-    <t>cookies, candy, crackers, cereals</t>
-  </si>
-  <si>
-    <t>not cause</t>
-  </si>
-  <si>
-    <t>sugar</t>
-  </si>
-  <si>
-    <t>obesity</t>
-  </si>
-  <si>
-    <t>isGoodFor</t>
-  </si>
-  <si>
-    <t>joints</t>
-  </si>
-  <si>
-    <t>healthy</t>
-  </si>
-  <si>
-    <t>sport</t>
-  </si>
-  <si>
-    <t>not isBadFor</t>
-  </si>
-  <si>
-    <t>running</t>
-  </si>
-  <si>
-    <t>shoulder pain</t>
-  </si>
-  <si>
-    <t>korean food</t>
-  </si>
-  <si>
-    <t>cream</t>
-  </si>
-  <si>
-    <t>causes</t>
-  </si>
-  <si>
-    <t>sports AND uses-upper-body-parts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eggs, meat </t>
-  </si>
-  <si>
-    <t>is</t>
-  </si>
-  <si>
-    <t>swimming</t>
-  </si>
-  <si>
-    <t>red meat</t>
-  </si>
-  <si>
-    <t>isA</t>
-  </si>
-  <si>
-    <t>kimbap, rabokki</t>
-  </si>
-  <si>
-    <t>contains</t>
-  </si>
-  <si>
-    <t>carbonara</t>
-  </si>
-  <si>
-    <t>prevents</t>
-  </si>
-  <si>
-    <t>Alzheimers</t>
-  </si>
-  <si>
-    <t>nuts, blueberries, strawberries</t>
-  </si>
-  <si>
-    <t>cancer, Alzheimers</t>
-  </si>
-  <si>
-    <t>nuts, olive oil, cococunt oil</t>
-  </si>
-  <si>
-    <t>fish, whole grains, green leafy vegetables, olives, nuts</t>
-  </si>
-  <si>
-    <t>alcohol, obesity, no-sport, tobacco</t>
-  </si>
-  <si>
-    <t>lowVitamin</t>
-  </si>
-  <si>
-    <t>hairLoss</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>successor atom</t>
+    <t>Alcohol, obesity and physical inactivity are all preventable causesCondition of cancer along with tobacco.</t>
+  </si>
+  <si>
+    <t>not sportCausesInjury</t>
+  </si>
+  <si>
+    <t>preventsCondition</t>
+  </si>
+  <si>
+    <t>CausesNutrientState</t>
+  </si>
+  <si>
+    <t>HealthyNutritionState</t>
   </si>
 </sst>
 </file>
@@ -301,7 +292,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -317,7 +308,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -616,7 +607,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,19 +624,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G1" s="2"/>
     </row>
@@ -660,13 +651,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -674,19 +665,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -694,19 +685,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
@@ -714,19 +705,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -734,19 +725,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -754,19 +745,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -774,19 +765,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -794,19 +785,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -814,19 +805,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -834,19 +825,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -854,19 +845,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -874,39 +865,39 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -914,19 +905,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
         <v>64</v>
       </c>
-      <c r="E15" t="s">
-        <v>59</v>
-      </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -934,19 +925,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -954,19 +945,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweet the word cancer is finally correct
</commit_message>
<xml_diff>
--- a/Agent/tweet_db.xlsx
+++ b/Agent/tweet_db.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hibaa\Documents\UU\Year 1\Q1\Intelligent Agents\IA\Agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D685ED-0AE6-4925-9DE0-A26F68C46988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05D0EA8D-9FD9-4191-932D-3E446B7AA59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,16 +41,53 @@
     <t>UserID</t>
   </si>
   <si>
+    <t>UserName</t>
+  </si>
+  <si>
     <t>Tweet</t>
   </si>
   <si>
+    <t>predecessor atom</t>
+  </si>
+  <si>
+    <t>relation</t>
+  </si>
+  <si>
+    <t>successor atom</t>
+  </si>
+  <si>
+    <t>"@bigfatsurprise"</t>
+  </si>
+  <si>
     <t>Headline needs fixing. Study shows a possible link between "ultra-processed" foods and cancer. "Ultra-processed" is dominated by packaged, cookies, crackers, cereals, candy--which are all mostly sugar+ grains+veg oil. These foods are more likely to cause cancer. evidence suggests</t>
   </si>
   <si>
-    <t>"@bigfatsurprise"</t>
+    <t>Cookies, Candy</t>
+  </si>
+  <si>
+    <t>causesCondition</t>
+  </si>
+  <si>
+    <t>cancer</t>
   </si>
   <si>
     <t>"@wellness_hc"</t>
+  </si>
+  <si>
+    <t>Does eating cake, cookies &amp; sweets cause breast cancer?
+There is no evidence that sugar consumption causesCondition breast cancer - or any other type of cancer. It is true that being overweight can increase your breast cancer risk. Avoiding sugary foods is better for your health!</t>
+  </si>
+  <si>
+    <t>highSugars</t>
+  </si>
+  <si>
+    <t>preventsCondition</t>
+  </si>
+  <si>
+    <t>obesity</t>
+  </si>
+  <si>
+    <t>"@willnewton"</t>
   </si>
   <si>
     <t>15-20 minutes a day working on your mobility issues could change your life.
@@ -61,125 +98,118 @@
 Mobility is magic.</t>
   </si>
   <si>
-    <t>"@willnewton"</t>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>not sportCausesInjury</t>
+  </si>
+  <si>
+    <t>Joint</t>
+  </si>
+  <si>
+    <t>"@chrisboettcher9"</t>
   </si>
   <si>
     <t xml:space="preserve">Running isn't bad for your knees. Weak hips, ankles, and feet are.  </t>
   </si>
   <si>
-    <t>"@chrisboettcher9"</t>
+    <t>Running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joint </t>
+  </si>
+  <si>
+    <t>"@drezekieloburu"</t>
   </si>
   <si>
     <t>Pain in the shoulder suggests a shoulder injury which is more common in athletes participating in sports such as swimming, tennis, pitching and weightlifting. The injuries are caused due to the over usage or repetitive motion of the arms.</t>
   </si>
   <si>
-    <t>"@drezekieloburu"</t>
+    <t>Sport AND usesBodyPart VALUE UpperBodyPart</t>
+  </si>
+  <si>
+    <t>sportCausesInjury</t>
+  </si>
+  <si>
+    <t>Shoulder injury</t>
+  </si>
+  <si>
+    <t>"@imaginephysio"</t>
   </si>
   <si>
     <t>Shoulder injury is the most common competitive swimming injury. It affects up to 90% of competitive swimmers</t>
   </si>
   <si>
-    <t>"@imaginephysio"</t>
+    <t>swimming</t>
+  </si>
+  <si>
+    <t>"@jason_muthomi"</t>
   </si>
   <si>
     <t>Eggs and red meat are healthy foods and should be eaten in plenty without fear.</t>
   </si>
   <si>
-    <t>"@jason_muthomi"</t>
+    <t xml:space="preserve">Egg, Meat </t>
+  </si>
+  <si>
+    <t>CausesNutrientState</t>
+  </si>
+  <si>
+    <t>HealthyNutritionState</t>
+  </si>
+  <si>
+    <t>"@Eric_Conn"</t>
   </si>
   <si>
     <t>Red meat is the ultimate superfood.</t>
   </si>
   <si>
-    <t>"@Eric_Conn"</t>
+    <t>Beef, lamb</t>
+  </si>
+  <si>
+    <t>"@joydielle"</t>
   </si>
   <si>
     <t>korean food with my best friends!! rabokki, dumplings and kimbap</t>
   </si>
   <si>
-    <t>"@joydielle"</t>
+    <t>kimbap, rabokki</t>
+  </si>
+  <si>
+    <t>isA</t>
+  </si>
+  <si>
+    <t>korean food</t>
+  </si>
+  <si>
+    <t>"@AnthraxAndrew"</t>
   </si>
   <si>
     <t>I'm going to make carbonara with cream.</t>
   </si>
   <si>
-    <t>"@AnthraxAndrew"</t>
+    <t>carbonara</t>
+  </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>cream</t>
+  </si>
+  <si>
+    <t>"@WebMD"</t>
   </si>
   <si>
     <t>Did you know both nuts and berries have been linked to better brain health? Blueberries and strawberries, in particular, help keep your brain working at its best and may slow symptoms linked to Alzheimer's</t>
   </si>
   <si>
-    <t>"@WebMD"</t>
+    <t>Nuts, Strawberry, blueberries</t>
+  </si>
+  <si>
+    <t>Alzheimer's</t>
   </si>
   <si>
     <t>"@drdenwalker"</t>
-  </si>
-  <si>
-    <t>Research shows that a Mediterranean-style diet rich in fish, whole grains, green leafy vegetables, olives, and nuts helps maintain brain health and may reduce the risk of Alzheimer’s disease.</t>
-  </si>
-  <si>
-    <t>"@VitaminsMemory"</t>
-  </si>
-  <si>
-    <t>"@thehealthbot"</t>
-  </si>
-  <si>
-    <t>A lack of the right #nutrients including #vitamins A, C, D and E, #zinc, B vitamins, #iron, #biotin, #protein and essential fatty acids may slow down hair growth or even cause hair loss.</t>
-  </si>
-  <si>
-    <t>"@recipeiq"</t>
-  </si>
-  <si>
-    <t>predecessor atom</t>
-  </si>
-  <si>
-    <t>relation</t>
-  </si>
-  <si>
-    <t>obesity</t>
-  </si>
-  <si>
-    <t>korean food</t>
-  </si>
-  <si>
-    <t>cream</t>
-  </si>
-  <si>
-    <t>swimming</t>
-  </si>
-  <si>
-    <t>isA</t>
-  </si>
-  <si>
-    <t>kimbap, rabokki</t>
-  </si>
-  <si>
-    <t>carbonara</t>
-  </si>
-  <si>
-    <t>alcohol, obesity, no-sport, tobacco</t>
-  </si>
-  <si>
-    <t>lowVitamin</t>
-  </si>
-  <si>
-    <t>hairLoss</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>successor atom</t>
-  </si>
-  <si>
-    <t>Contains</t>
-  </si>
-  <si>
-    <t>Does eating cake, cookies &amp; sweets cause breast cancer?
-There is no evidence that sugar consumption causesCondition breast cancer - or any other type of cancer. It is true that being overweight can increase your breast cancer risk. Avoiding sugary foods is better for your health!</t>
-  </si>
-  <si>
-    <t>causesCondition</t>
   </si>
   <si>
     <t>Reasons why you should include Nuts, Seeds, Olive Oil, Coconut Oil
@@ -189,77 +219,47 @@
 RT and Share</t>
   </si>
   <si>
+    <t>Nuts, olive oil, coconut oil</t>
+  </si>
+  <si>
+    <t>cancer, Alzheimer's</t>
+  </si>
+  <si>
+    <t>"@VitaminsMemory"</t>
+  </si>
+  <si>
+    <t>Research shows that a Mediterranean-style diet rich in fish, whole grains, green leafy vegetables, olives, and nuts helps maintain brain health and may reduce the risk of Alzheimer’s disease.</t>
+  </si>
+  <si>
+    <t>Fish, whole grains, green leafy vegetables, olives, Nuts</t>
+  </si>
+  <si>
+    <t>"@thehealthbot"</t>
+  </si>
+  <si>
     <t>Alcohol, obesity and physical inactivity are all preventable causesCondition of cancer along with tobacco.</t>
   </si>
   <si>
-    <t>not sportCausesInjury</t>
-  </si>
-  <si>
-    <t>preventsCondition</t>
-  </si>
-  <si>
-    <t>CausesNutrientState</t>
-  </si>
-  <si>
-    <t>HealthyNutritionState</t>
-  </si>
-  <si>
-    <t>Cookies, Candy</t>
-  </si>
-  <si>
-    <t>Cancer</t>
-  </si>
-  <si>
-    <t>highSugars</t>
-  </si>
-  <si>
-    <t>Sport</t>
-  </si>
-  <si>
-    <t>Joint</t>
-  </si>
-  <si>
-    <t>Running</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joint </t>
-  </si>
-  <si>
-    <t>Sport AND usesBodyPart VALUE UpperBodyPart</t>
-  </si>
-  <si>
-    <t>sportCausesInjury</t>
-  </si>
-  <si>
-    <t>Shoulder injury</t>
-  </si>
-  <si>
-    <t>Alzheimer's</t>
-  </si>
-  <si>
-    <t>Cancer, Alzheimer's</t>
-  </si>
-  <si>
-    <t>Fish, whole grains, green leafy vegetables, olives, Nuts</t>
-  </si>
-  <si>
-    <t>Nuts, olive oil, coconut oil</t>
-  </si>
-  <si>
-    <t>Nuts, Strawberry, blueberries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egg, Meat </t>
-  </si>
-  <si>
-    <t>Beef, lamb</t>
+    <t>alcohol, obesity, no-sport, tobacco</t>
+  </si>
+  <si>
+    <t>"@recipeiq"</t>
+  </si>
+  <si>
+    <t>A lack of the right #nutrients including #vitamins A, C, D and E, #zinc, B vitamins, #iron, #biotin, #protein and essential fatty acids may slow down hair growth or even cause hair loss.</t>
+  </si>
+  <si>
+    <t>lowVitamin</t>
+  </si>
+  <si>
+    <t>hairLoss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,7 +298,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -612,358 +612,358 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="91.15" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="100.9">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="100.9">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="129.6">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.9">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="72">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.15">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.9">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.9">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="72">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="129.6">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="57.6">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.15">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="57.6">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct ontologies and stories naming
</commit_message>
<xml_diff>
--- a/Agent/tweet_db.xlsx
+++ b/Agent/tweet_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hibaa\Documents\UU\Year 1\Q1\Intelligent Agents\IA\Agent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IA\IA\Agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05D0EA8D-9FD9-4191-932D-3E446B7AA59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F266F15-B16A-4DC5-9FD9-84A70A7B34C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>UserID</t>
   </si>
@@ -78,13 +78,7 @@
 There is no evidence that sugar consumption causesCondition breast cancer - or any other type of cancer. It is true that being overweight can increase your breast cancer risk. Avoiding sugary foods is better for your health!</t>
   </si>
   <si>
-    <t>highSugars</t>
-  </si>
-  <si>
     <t>preventsCondition</t>
-  </si>
-  <si>
-    <t>obesity</t>
   </si>
   <si>
     <t>"@willnewton"</t>
@@ -125,9 +119,6 @@
     <t>Pain in the shoulder suggests a shoulder injury which is more common in athletes participating in sports such as swimming, tennis, pitching and weightlifting. The injuries are caused due to the over usage or repetitive motion of the arms.</t>
   </si>
   <si>
-    <t>Sport AND usesBodyPart VALUE UpperBodyPart</t>
-  </si>
-  <si>
     <t>sportCausesInjury</t>
   </si>
   <si>
@@ -140,9 +131,6 @@
     <t>Shoulder injury is the most common competitive swimming injury. It affects up to 90% of competitive swimmers</t>
   </si>
   <si>
-    <t>swimming</t>
-  </si>
-  <si>
     <t>"@jason_muthomi"</t>
   </si>
   <si>
@@ -152,9 +140,6 @@
     <t xml:space="preserve">Egg, Meat </t>
   </si>
   <si>
-    <t>CausesNutrientState</t>
-  </si>
-  <si>
     <t>HealthyNutritionState</t>
   </si>
   <si>
@@ -164,46 +149,25 @@
     <t>Red meat is the ultimate superfood.</t>
   </si>
   <si>
-    <t>Beef, lamb</t>
-  </si>
-  <si>
     <t>"@joydielle"</t>
   </si>
   <si>
     <t>korean food with my best friends!! rabokki, dumplings and kimbap</t>
   </si>
   <si>
-    <t>kimbap, rabokki</t>
-  </si>
-  <si>
     <t>isA</t>
   </si>
   <si>
-    <t>korean food</t>
-  </si>
-  <si>
     <t>"@AnthraxAndrew"</t>
   </si>
   <si>
     <t>I'm going to make carbonara with cream.</t>
   </si>
   <si>
-    <t>carbonara</t>
-  </si>
-  <si>
-    <t>Contains</t>
-  </si>
-  <si>
-    <t>cream</t>
-  </si>
-  <si>
     <t>"@WebMD"</t>
   </si>
   <si>
     <t>Did you know both nuts and berries have been linked to better brain health? Blueberries and strawberries, in particular, help keep your brain working at its best and may slow symptoms linked to Alzheimer's</t>
-  </si>
-  <si>
-    <t>Nuts, Strawberry, blueberries</t>
   </si>
   <si>
     <t>Alzheimer's</t>
@@ -219,47 +183,86 @@
 RT and Share</t>
   </si>
   <si>
-    <t>Nuts, olive oil, coconut oil</t>
-  </si>
-  <si>
-    <t>cancer, Alzheimer's</t>
-  </si>
-  <si>
     <t>"@VitaminsMemory"</t>
   </si>
   <si>
     <t>Research shows that a Mediterranean-style diet rich in fish, whole grains, green leafy vegetables, olives, and nuts helps maintain brain health and may reduce the risk of Alzheimer’s disease.</t>
   </si>
   <si>
-    <t>Fish, whole grains, green leafy vegetables, olives, Nuts</t>
-  </si>
-  <si>
     <t>"@thehealthbot"</t>
   </si>
   <si>
     <t>Alcohol, obesity and physical inactivity are all preventable causesCondition of cancer along with tobacco.</t>
   </si>
   <si>
-    <t>alcohol, obesity, no-sport, tobacco</t>
-  </si>
-  <si>
     <t>"@recipeiq"</t>
   </si>
   <si>
     <t>A lack of the right #nutrients including #vitamins A, C, D and E, #zinc, B vitamins, #iron, #biotin, #protein and essential fatty acids may slow down hair growth or even cause hair loss.</t>
   </si>
   <si>
-    <t>lowVitamin</t>
-  </si>
-  <si>
-    <t>hairLoss</t>
+    <t>causesNutrientState</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t>Sport AND UsesBodyPart VALUE UpperBodyPart</t>
+  </si>
+  <si>
+    <t>Swimming</t>
+  </si>
+  <si>
+    <t>Beef, Lamb</t>
+  </si>
+  <si>
+    <t>Kimbap, Rabokki</t>
+  </si>
+  <si>
+    <t>Carbonara</t>
+  </si>
+  <si>
+    <t>Cream</t>
+  </si>
+  <si>
+    <t>KoreanFood</t>
+  </si>
+  <si>
+    <t>Nuts, Strawberry, Blueberries</t>
+  </si>
+  <si>
+    <t>Nuts, OliveOil, CoconutOil</t>
+  </si>
+  <si>
+    <t>Fish, WholeGrains, GreenLeafyVegetables, Olives, Nuts</t>
+  </si>
+  <si>
+    <t>Alcohol, Obesity, NoSport, Tobacco</t>
+  </si>
+  <si>
+    <t>LowVitamin</t>
+  </si>
+  <si>
+    <t>HairLoss</t>
+  </si>
+  <si>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t>Cancer, Alzheimer's</t>
+  </si>
+  <si>
+    <t>HighSugars</t>
+  </si>
+  <si>
+    <t>Obesity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,20 +615,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +649,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="91.15" customHeight="1">
+    <row r="2" spans="1:7" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -666,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="100.9">
+    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -677,16 +680,16 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="100.9">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -697,273 +700,273 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="129.6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.9">
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="72">
+    </row>
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.15">
+    </row>
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="72">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="129.6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="43.15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="57.6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugs in twitter db fixed
</commit_message>
<xml_diff>
--- a/Agent/tweet_db.xlsx
+++ b/Agent/tweet_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IA\IA\Agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F266F15-B16A-4DC5-9FD9-84A70A7B34C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42E9C40-5C53-44F0-B774-647F12964CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>UserID</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>causesCondition</t>
-  </si>
-  <si>
-    <t>cancer</t>
   </si>
   <si>
     <t>"@wellness_hc"</t>
@@ -95,9 +92,6 @@
     <t>Sport</t>
   </si>
   <si>
-    <t>not sportCausesInjury</t>
-  </si>
-  <si>
     <t>Joint</t>
   </si>
   <si>
@@ -117,12 +111,6 @@
   </si>
   <si>
     <t>Pain in the shoulder suggests a shoulder injury which is more common in athletes participating in sports such as swimming, tennis, pitching and weightlifting. The injuries are caused due to the over usage or repetitive motion of the arms.</t>
-  </si>
-  <si>
-    <t>sportCausesInjury</t>
-  </si>
-  <si>
-    <t>Shoulder injury</t>
   </si>
   <si>
     <t>"@imaginephysio"</t>
@@ -207,9 +195,6 @@
     <t>contains</t>
   </si>
   <si>
-    <t>Sport AND UsesBodyPart VALUE UpperBodyPart</t>
-  </si>
-  <si>
     <t>Swimming</t>
   </si>
   <si>
@@ -256,6 +241,18 @@
   </si>
   <si>
     <t>Obesity</t>
+  </si>
+  <si>
+    <t>causesInjury</t>
+  </si>
+  <si>
+    <t>notCausesInjury</t>
+  </si>
+  <si>
+    <t>Tennis</t>
+  </si>
+  <si>
+    <t>Shoulder</t>
   </si>
 </sst>
 </file>
@@ -613,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +663,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -674,19 +671,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -694,19 +691,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
@@ -714,19 +711,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -734,19 +731,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -754,219 +751,239 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>